<commit_message>
Gerador atualizado com nivel educacional
</commit_message>
<xml_diff>
--- a/perfis_generated_openpyxl.xlsx
+++ b/perfis_generated_openpyxl.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G101"/>
+  <dimension ref="A1:H101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -449,10 +449,15 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
+          <t>Educação</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
           <t>CPF</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>CEP</t>
         </is>
@@ -464,11 +469,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Tatiane Ferreira</t>
+          <t>Vanessa Mendes Ramos Gonçalves</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>20</v>
+        <v>52</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -477,17 +482,22 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>546.986.390-50</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>891783891</t>
+          <t>840.040.580-31</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>735931870</t>
         </is>
       </c>
     </row>
@@ -497,30 +507,35 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Fábio Vieira Pessoa</t>
+          <t>Vanessa Santos Martins</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>923.622.410-50</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>253830283</t>
+          <t>513.769.110-00</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>437371199</t>
         </is>
       </c>
     </row>
@@ -530,30 +545,35 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Roberto Borges Nogueira Cavalcanti</t>
+          <t>Larissa Araújo Lima</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>212.269.980-97</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>114870724</t>
+          <t>708.211.000-68</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>696826907</t>
         </is>
       </c>
     </row>
@@ -563,30 +583,35 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Felipe Borges Freitas</t>
+          <t>Ricardo Giovanni Oliveira Freitas Ribeiro</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Não-Binário</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branco(a)</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>868.665.000-79</t>
+          <t>Superior completo</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>054399389</t>
+          <t>858.530.260-70</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>558643753</t>
         </is>
       </c>
     </row>
@@ -596,30 +621,35 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Priscila Alves</t>
+          <t>André Araújo</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>269.068.190-03</t>
+          <t>Superior completo</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>261506950</t>
+          <t>914.797.510-57</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>032386065</t>
         </is>
       </c>
     </row>
@@ -629,11 +659,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Luis Ramos Castro</t>
+          <t>Leonardo Andrade Pereira</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -642,17 +672,22 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>860.665.080-32</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>866020036</t>
+          <t>085.587.130-06</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>108151471</t>
         </is>
       </c>
     </row>
@@ -662,30 +697,35 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Juliana Rocha Ribeira</t>
+          <t>Gilberto Ribeira Monteiro</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>974.639.050-39</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>689141582</t>
+          <t>875.771.360-00</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>911398703</t>
         </is>
       </c>
     </row>
@@ -695,30 +735,35 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Alexandre Machado Cardoso Fernandes Campos</t>
+          <t>Flávia Sousa Nunes</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>745.079.220-62</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>516403680</t>
+          <t>724.826.840-21</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>327634327</t>
         </is>
       </c>
     </row>
@@ -728,30 +773,35 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Tatiana Martins Correia Lima</t>
+          <t>Roberto Vieira</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>911.691.470-89</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>569451448</t>
+          <t>273.639.850-57</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>316862767</t>
         </is>
       </c>
     </row>
@@ -761,11 +811,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Paulo Moraes</t>
+          <t>Márcio Carvalho Lopes</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -779,12 +829,17 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>692.721.920-05</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>988814908</t>
+          <t>641.907.670-69</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>160715921</t>
         </is>
       </c>
     </row>
@@ -794,11 +849,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Sueli Barbosa Almeida</t>
+          <t>Eduarda Costa</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -812,12 +867,17 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>948.733.770-99</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>616282767</t>
+          <t>682.985.220-01</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>712941687</t>
         </is>
       </c>
     </row>
@@ -827,30 +887,35 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Roberto Ribeira Carvalho</t>
+          <t>Lucas Alves</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>27</v>
+        <v>6</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Não-Binário</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Pardo(a)</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>237.876.820-66</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>327767612</t>
+          <t>353.387.880-55</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>295414373</t>
         </is>
       </c>
     </row>
@@ -860,11 +925,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Fábio Oliveira Moraes</t>
+          <t>Renato Arnaldo Gouveia</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -873,17 +938,22 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>556.947.080-83</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>800046436</t>
+          <t>433.580.710-49</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>373552401</t>
         </is>
       </c>
     </row>
@@ -893,30 +963,35 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>César Oliveira Moraes</t>
+          <t>Valéria Simone Lima Fernandes</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>171.353.500-90</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>504748793</t>
+          <t>409.235.280-83</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>432581667</t>
         </is>
       </c>
     </row>
@@ -926,30 +1001,35 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Felipe Rafael Rocha Rocha Ribeira</t>
+          <t>Carolina Lorena Cavalcanti Silva</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>802.307.680-91</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>089803051</t>
+          <t>668.982.720-80</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>838752449</t>
         </is>
       </c>
     </row>
@@ -959,11 +1039,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Eduardo Andrade</t>
+          <t>Vicente Mendes Ferreira</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -977,12 +1057,17 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>424.183.650-00</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>707543322</t>
+          <t>887.569.010-38</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>262550978</t>
         </is>
       </c>
     </row>
@@ -992,30 +1077,35 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Natália Correia</t>
+          <t>Alberto Nascimento Almeida Cardoso Carvalho</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>39</v>
+        <v>2</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>883.757.170-45</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>250150360</t>
+          <t>147.738.460-03</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>227737486</t>
         </is>
       </c>
     </row>
@@ -1025,11 +1115,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Sueli Andrade Pessoa</t>
+          <t>Sueli Mendes</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1038,17 +1128,22 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>220.708.810-32</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>139939879</t>
+          <t>161.910.290-04</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>414251792</t>
         </is>
       </c>
     </row>
@@ -1058,11 +1153,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ronaldo Fernando Nogueira Silveira Sousa Azevedo</t>
+          <t>Sergio Márcio Castro Machado Silva</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>49</v>
+        <v>23</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1076,12 +1171,17 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>208.222.310-85</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>288017916</t>
+          <t>420.850.560-59</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>266481675</t>
         </is>
       </c>
     </row>
@@ -1091,11 +1191,11 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Tatiana Laura Santana Dias</t>
+          <t>Amanda Dias Sousa</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
@@ -1104,17 +1204,22 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>736.783.190-92</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>098077607</t>
+          <t>830.161.640-78</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>582454050</t>
         </is>
       </c>
     </row>
@@ -1124,30 +1229,35 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Camila Ribeiro Pessoa Costa</t>
+          <t>Pedro Barros Santos Cavalcanti</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>920.121.140-67</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>890228820</t>
+          <t>642.943.080-44</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>751563947</t>
         </is>
       </c>
     </row>
@@ -1157,30 +1267,35 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Eduarda Cardoso Lopes</t>
+          <t>Marcelo Thiago Mendes Ferreira</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>308.535.130-23</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>624525667</t>
+          <t>486.499.850-76</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>032013529</t>
         </is>
       </c>
     </row>
@@ -1190,11 +1305,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Alexandre Nogueira Gomes</t>
+          <t>Fernando Gonçalves Pereira Pessoa Campos</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>48</v>
+        <v>13</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1203,17 +1318,22 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>844.227.640-80</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>781114328</t>
+          <t>454.088.970-28</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>218493741</t>
         </is>
       </c>
     </row>
@@ -1223,11 +1343,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Cecília Priscila Alves Andrade</t>
+          <t>Simone Ana Machado Moraes Andrade</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1241,12 +1361,17 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>177.942.250-43</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>130004475</t>
+          <t>727.022.380-76</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>115398536</t>
         </is>
       </c>
     </row>
@@ -1256,11 +1381,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Jessica Fernanda Oliveira Cavalcanti Ribeira</t>
+          <t>Amanda Helena Ferreira Almeida</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1269,17 +1394,22 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>021.495.240-15</t>
+          <t>Superior completo</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>290937730</t>
+          <t>160.102.800-87</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>376270147</t>
         </is>
       </c>
     </row>
@@ -1289,30 +1419,35 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Fernanda Lopes Nascimento</t>
+          <t>Wagner Alves Borges Machado</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>057.893.190-76</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>669405074</t>
+          <t>541.772.380-07</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>794495135</t>
         </is>
       </c>
     </row>
@@ -1322,30 +1457,35 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Márcio Daniel Dias Almeida</t>
+          <t>Helena Lima Andrade</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>632.841.220-79</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>818162779</t>
+          <t>429.240.180-21</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>755807288</t>
         </is>
       </c>
     </row>
@@ -1355,30 +1495,35 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Geraldo Nunes</t>
+          <t>Lorena Thais Machado Cardoso</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>851.015.070-24</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>382707360</t>
+          <t>789.383.970-84</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>405148551</t>
         </is>
       </c>
     </row>
@@ -1388,30 +1533,35 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Cristina Dias Vieira</t>
+          <t>Guilherme Fernando Lima Dias</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>109.716.100-53</t>
+          <t>Superior completo</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>750599560</t>
+          <t>990.879.750-66</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>557945670</t>
         </is>
       </c>
     </row>
@@ -1421,11 +1571,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Fernanda Alves Nunes</t>
+          <t>Ana Nascimento Costa</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1439,12 +1589,17 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>260.540.560-50</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>462129995</t>
+          <t>012.152.930-46</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>719115070</t>
         </is>
       </c>
     </row>
@@ -1454,30 +1609,35 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Priscila Roberta Silveira</t>
+          <t>Gustavo Santos Moraes</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>364.111.300-86</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>299271474</t>
+          <t>323.680.570-64</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>632595583</t>
         </is>
       </c>
     </row>
@@ -1487,7 +1647,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Amanda Campos Barbosa</t>
+          <t>Vanessa Valéria Sousa</t>
         </is>
       </c>
       <c r="C33" t="n">
@@ -1500,17 +1660,22 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>130.025.090-94</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>584382272</t>
+          <t>653.561.780-77</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>747400143</t>
         </is>
       </c>
     </row>
@@ -1520,11 +1685,11 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Maria Rodrigues Cardoso</t>
+          <t>Eduarda Santos</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
@@ -1533,17 +1698,22 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>866.204.540-54</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>303123502</t>
+          <t>938.610.320-66</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>569265739</t>
         </is>
       </c>
     </row>
@@ -1553,30 +1723,35 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Cecília Vieira Rocha</t>
+          <t>Gilberto Pedro Monteiro Rocha Dias</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>594.527.240-05</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>602459684</t>
+          <t>212.796.350-45</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>909680243</t>
         </is>
       </c>
     </row>
@@ -1586,11 +1761,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Fernando Barros Lopes</t>
+          <t>Ricardo Pires Oliveira</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>28</v>
+        <v>44</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1599,17 +1774,22 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>154.542.490-09</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>523069829</t>
+          <t>650.324.960-81</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>863703824</t>
         </is>
       </c>
     </row>
@@ -1619,11 +1799,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Carlos Freitas Santos</t>
+          <t>Thiago Monteiro Pires</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1632,17 +1812,22 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>050.247.650-87</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>358803031</t>
+          <t>327.376.110-59</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>099276398</t>
         </is>
       </c>
     </row>
@@ -1652,11 +1837,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Vicente César Lopes Ramos</t>
+          <t>Daniel Mendes</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>38</v>
+        <v>17</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -1665,17 +1850,22 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>781.994.330-00</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>405450592</t>
+          <t>967.752.660-06</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>342341833</t>
         </is>
       </c>
     </row>
@@ -1685,11 +1875,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Jéssica Vieira</t>
+          <t>Carolina Silveira Campos Ramos Martins</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -1703,12 +1893,17 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>811.819.170-26</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>729947011</t>
+          <t>067.243.200-54</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>317516768</t>
         </is>
       </c>
     </row>
@@ -1718,30 +1913,35 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Gustavo Lima Santos Cardoso Nascimento</t>
+          <t>Mariana Campos Cardoso</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>503.405.590-20</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>157206490</t>
+          <t>016.342.870-02</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>799418783</t>
         </is>
       </c>
     </row>
@@ -1751,11 +1951,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Nathalia Isabela Cavalcanti Oliveira Pessoa</t>
+          <t>Larissa Moraes Martins</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -1769,12 +1969,17 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>729.419.280-49</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>427928073</t>
+          <t>620.562.560-10</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>879367550</t>
         </is>
       </c>
     </row>
@@ -1784,30 +1989,35 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Roberta Camila Cavalcanti</t>
+          <t>Caio Ribeira Nascimento</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>140.331.030-07</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>890626734</t>
+          <t>684.395.320-40</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>575316960</t>
         </is>
       </c>
     </row>
@@ -1817,30 +2027,35 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Aline Priscila Ribeira Mendes</t>
+          <t>Fábio Barbosa Gomes Dias</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>366.127.830-44</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>584372082</t>
+          <t>369.538.060-87</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>596135162</t>
         </is>
       </c>
     </row>
@@ -1850,30 +2065,35 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Luis Freitas Pessoa</t>
+          <t>Thais Helena Martins Rocha</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>001.009.560-84</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>242831640</t>
+          <t>071.778.010-49</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>475394399</t>
         </is>
       </c>
     </row>
@@ -1883,11 +2103,11 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Alexandre Sousa</t>
+          <t>Rafael Pires Andrade</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
@@ -1901,12 +2121,17 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>145.894.690-81</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>337976311</t>
+          <t>374.568.940-27</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>928857577</t>
         </is>
       </c>
     </row>
@@ -1916,11 +2141,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Larissa Machado Borges</t>
+          <t>Lorena Carolina Ribeira Sousa</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>4</v>
+        <v>36</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -1934,12 +2159,17 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>020.260.980-42</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>049672434</t>
+          <t>806.338.890-91</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>322825093</t>
         </is>
       </c>
     </row>
@@ -1949,11 +2179,11 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Roberto Lima Costa</t>
+          <t>Leandro Martins</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
@@ -1962,17 +2192,22 @@
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>664.892.310-50</t>
+          <t>Fundamental completo</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>473000674</t>
+          <t>351.560.870-27</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>701013114</t>
         </is>
       </c>
     </row>
@@ -1982,11 +2217,11 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Alberto Rocha Martins</t>
+          <t>Geraldo Pereira Nascimento Lopes Gonçalves</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
@@ -1995,17 +2230,22 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>475.818.070-96</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>358986789</t>
+          <t>627.237.350-36</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>636476466</t>
         </is>
       </c>
     </row>
@@ -2015,11 +2255,11 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Álvaro Ferreira</t>
+          <t>Luis Moraes Costa</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
@@ -2028,17 +2268,22 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>583.611.920-18</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>885801071</t>
+          <t>496.741.360-96</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>387923208</t>
         </is>
       </c>
     </row>
@@ -2048,11 +2293,11 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Marcelo Pereira</t>
+          <t>Lucas Rocha Nogueira</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>14</v>
+        <v>54</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
@@ -2061,17 +2306,22 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>137.777.940-82</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>787477400</t>
+          <t>027.266.940-71</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>233842869</t>
         </is>
       </c>
     </row>
@@ -2081,30 +2331,35 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Fernanda Lopes Pinto</t>
+          <t>José Ribeira Machado</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>232.075.820-87</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>640639240</t>
+          <t>371.468.740-87</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>889682013</t>
         </is>
       </c>
     </row>
@@ -2114,30 +2369,35 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Carlos Cavalcanti Mendes Lima</t>
+          <t>Priscila Carvalho Campos</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>017.809.840-06</t>
+          <t>Fundamental completo</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>329660858</t>
+          <t>554.326.730-45</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>906812106</t>
         </is>
       </c>
     </row>
@@ -2147,11 +2407,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Valéria Nascimento Santos</t>
+          <t>Elaine Costa</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -2160,17 +2420,22 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>126.859.920-49</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>701449179</t>
+          <t>280.417.060-88</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>518108814</t>
         </is>
       </c>
     </row>
@@ -2180,11 +2445,11 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Larissa Lima Mendes Ribeira</t>
+          <t>Bianca Lopes</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
@@ -2193,17 +2458,22 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>583.383.050-81</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>342131589</t>
+          <t>081.171.530-25</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>537203665</t>
         </is>
       </c>
     </row>
@@ -2213,30 +2483,35 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Jéssica Ramos Almeida</t>
+          <t>Fernando Pedro Pinto Pinto</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>065.032.630-07</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>409113786</t>
+          <t>999.808.590-08</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>645193816</t>
         </is>
       </c>
     </row>
@@ -2246,11 +2521,11 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Roberto Leandro Moraes Cardoso</t>
+          <t>Hugo José Fernandes Moraes</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -2259,17 +2534,22 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>031.573.180-04</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>966543062</t>
+          <t>133.918.080-47</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>632429832</t>
         </is>
       </c>
     </row>
@@ -2279,30 +2559,35 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Isabela Carvalho Ramos Martins</t>
+          <t>Guilherme Lima</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>906.550.850-33</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>612617182</t>
+          <t>167.147.640-90</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>337153744</t>
         </is>
       </c>
     </row>
@@ -2312,11 +2597,11 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Eduarda Cavalcanti Silveira</t>
+          <t>Cecília Renata Gonçalves</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -2325,17 +2610,22 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>276.863.970-25</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>580977529</t>
+          <t>628.327.630-06</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>350071017</t>
         </is>
       </c>
     </row>
@@ -2345,30 +2635,35 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>João Miguel Gonçalves</t>
+          <t>Ricardo Costa Barbosa Pereira Pinto</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Não-Binário</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Pardo(a)</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>205.287.140-31</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>736372155</t>
+          <t>567.929.410-93</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>537084321</t>
         </is>
       </c>
     </row>
@@ -2378,11 +2673,11 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Priscila Gomes Mendes</t>
+          <t>Jessica Oliveira Lopes Fernandes</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -2396,12 +2691,17 @@
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>207.847.440-17</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>411179195</t>
+          <t>199.027.830-23</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>464241410</t>
         </is>
       </c>
     </row>
@@ -2411,30 +2711,35 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Sueli Carvalho Azevedo Cavalcanti Mendes</t>
+          <t>Armando Fernando Martins</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>899.080.520-12</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>133009164</t>
+          <t>103.661.950-85</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>187210039</t>
         </is>
       </c>
     </row>
@@ -2444,30 +2749,35 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Rosana Ribeira Freitas</t>
+          <t>Luis Borges Carvalho</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>994.833.850-24</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>554283051</t>
+          <t>991.304.290-99</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>223128737</t>
         </is>
       </c>
     </row>
@@ -2477,11 +2787,11 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Aline Oliveira Lima</t>
+          <t>Laura Nunes</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -2490,17 +2800,22 @@
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>178.770.210-38</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>453702257</t>
+          <t>424.327.090-20</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>870158300</t>
         </is>
       </c>
     </row>
@@ -2510,11 +2825,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Thais Nunes Carvalho</t>
+          <t>Larissa Machado Campos</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -2523,17 +2838,22 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>757.240.780-31</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>380772141</t>
+          <t>564.451.720-91</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>848184863</t>
         </is>
       </c>
     </row>
@@ -2543,30 +2863,35 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Karla Carolina Moraes</t>
+          <t>César Carlos Campos</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>46</v>
+        <v>16</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>157.450.740-00</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>433095248</t>
+          <t>475.091.670-60</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>785714726</t>
         </is>
       </c>
     </row>
@@ -2576,30 +2901,35 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Eduarda Jéssica Lopes</t>
+          <t>César Correia Machado Machado</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>976.252.740-20</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>192528350</t>
+          <t>161.872.520-39</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>686016292</t>
         </is>
       </c>
     </row>
@@ -2609,30 +2939,35 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Gilberto Santana Alves</t>
+          <t>Luiza Camila Cavalcanti</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>452.963.220-29</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>439049841</t>
+          <t>372.584.640-50</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>076645441</t>
         </is>
       </c>
     </row>
@@ -2642,30 +2977,35 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Aline Nunes Pinto</t>
+          <t>Anderson Mendes</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>784.298.750-50</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>699819775</t>
+          <t>418.447.840-96</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>853346523</t>
         </is>
       </c>
     </row>
@@ -2675,11 +3015,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Felipe Anderson Mendes Santos Gomes</t>
+          <t>Antônio Sousa</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -2688,17 +3028,22 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>701.004.710-30</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>471325360</t>
+          <t>816.117.100-90</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>965769279</t>
         </is>
       </c>
     </row>
@@ -2708,11 +3053,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Andressa Cátia Gonçalves Vieira Borges</t>
+          <t>Mônica Andrade Gomes</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -2721,17 +3066,22 @@
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>895.943.530-90</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>420925473</t>
+          <t>339.636.020-66</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>822223526</t>
         </is>
       </c>
     </row>
@@ -2741,11 +3091,11 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Elaine Isabela Cavalcanti</t>
+          <t>Rosana Almeida Silva Ribeiro</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -2754,17 +3104,22 @@
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>858.524.720-77</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>613082680</t>
+          <t>854.831.030-84</t>
+        </is>
+      </c>
+      <c r="H71" t="inlineStr">
+        <is>
+          <t>486246551</t>
         </is>
       </c>
     </row>
@@ -2774,30 +3129,35 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Amanda Fernandes</t>
+          <t>Guilherme Alves Cardoso</t>
         </is>
       </c>
       <c r="C72" t="n">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>152.653.140-24</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>824822389</t>
+          <t>795.955.240-18</t>
+        </is>
+      </c>
+      <c r="H72" t="inlineStr">
+        <is>
+          <t>679038979</t>
         </is>
       </c>
     </row>
@@ -2807,30 +3167,35 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Laura Gouveia</t>
+          <t>César Alves Ferreira</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>036.280.360-97</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>186417768</t>
+          <t>716.128.490-24</t>
+        </is>
+      </c>
+      <c r="H73" t="inlineStr">
+        <is>
+          <t>712727530</t>
         </is>
       </c>
     </row>
@@ -2840,11 +3205,11 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Carlos Machado Ribeiro</t>
+          <t>André Gouveia</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -2858,12 +3223,17 @@
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>188.046.790-93</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>012252653</t>
+          <t>296.266.070-33</t>
+        </is>
+      </c>
+      <c r="H74" t="inlineStr">
+        <is>
+          <t>949672051</t>
         </is>
       </c>
     </row>
@@ -2873,30 +3243,35 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Fábio Carlos Azevedo Gomes</t>
+          <t>Sueli Isabela Andrade Nunes</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>583.278.870-25</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>132121744</t>
+          <t>497.691.410-03</t>
+        </is>
+      </c>
+      <c r="H75" t="inlineStr">
+        <is>
+          <t>102046442</t>
         </is>
       </c>
     </row>
@@ -2906,11 +3281,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Márcia Mariana Mendes</t>
+          <t>Natália Lima Andrade</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -2924,12 +3299,17 @@
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>173.804.540-48</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>957513839</t>
+          <t>258.589.160-74</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>196066164</t>
         </is>
       </c>
     </row>
@@ -2939,11 +3319,11 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Marcelo Barros</t>
+          <t>Carlos Lucas Ribeiro Cardoso</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -2952,17 +3332,22 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>716.043.350-50</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>850555119</t>
+          <t>099.600.940-06</t>
+        </is>
+      </c>
+      <c r="H77" t="inlineStr">
+        <is>
+          <t>655405872</t>
         </is>
       </c>
     </row>
@@ -2972,30 +3357,35 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Isaac Ferreira Cardoso</t>
+          <t>Eduarda Sueli Vieira Rodrigues Ribeiro</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>006.039.380-78</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>811973131</t>
+          <t>505.715.850-35</t>
+        </is>
+      </c>
+      <c r="H78" t="inlineStr">
+        <is>
+          <t>856775474</t>
         </is>
       </c>
     </row>
@@ -3005,11 +3395,11 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Fernanda Larissa Borges Carvalho</t>
+          <t>Karla Cavalcanti Correia</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -3018,17 +3408,22 @@
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>607.314.240-42</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>110510974</t>
+          <t>637.288.780-06</t>
+        </is>
+      </c>
+      <c r="H79" t="inlineStr">
+        <is>
+          <t>188900833</t>
         </is>
       </c>
     </row>
@@ -3038,11 +3433,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Regina Cavalcanti Gomes</t>
+          <t>Tatiana Lopes</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -3056,12 +3451,17 @@
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>924.353.730-07</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>973625218</t>
+          <t>876.391.150-78</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>876596742</t>
         </is>
       </c>
     </row>
@@ -3071,11 +3471,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Tatiane Monteiro Pires Vieira Araújo</t>
+          <t>Brenda Borges Andrade</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -3089,12 +3489,17 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>352.610.820-05</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>207638331</t>
+          <t>669.195.860-88</t>
+        </is>
+      </c>
+      <c r="H81" t="inlineStr">
+        <is>
+          <t>796968100</t>
         </is>
       </c>
     </row>
@@ -3104,11 +3509,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Ricardo Carvalho Nascimento</t>
+          <t>Armando Carlos Lima Martins</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -3117,17 +3522,22 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>090.639.920-33</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>361138403</t>
+          <t>489.515.590-09</t>
+        </is>
+      </c>
+      <c r="H82" t="inlineStr">
+        <is>
+          <t>284307808</t>
         </is>
       </c>
     </row>
@@ -3137,30 +3547,35 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Marcelo Vicente Ferreira Dias Rodrigues</t>
+          <t>Fernanda Jessica Martins</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>241.082.160-08</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>804116273</t>
+          <t>782.225.890-75</t>
+        </is>
+      </c>
+      <c r="H83" t="inlineStr">
+        <is>
+          <t>067334167</t>
         </is>
       </c>
     </row>
@@ -3170,30 +3585,35 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Vanessa Patrícia Pereira Santos</t>
+          <t>Gilberto Costa</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>960.663.590-29</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>367687451</t>
+          <t>742.703.780-42</t>
+        </is>
+      </c>
+      <c r="H84" t="inlineStr">
+        <is>
+          <t>677738872</t>
         </is>
       </c>
     </row>
@@ -3203,11 +3623,11 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Eduarda Dias Almeida</t>
+          <t>Sandra Pereira Almeida</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>51</v>
+        <v>14</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -3221,12 +3641,17 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>854.228.510-72</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>033903708</t>
+          <t>533.643.360-83</t>
+        </is>
+      </c>
+      <c r="H85" t="inlineStr">
+        <is>
+          <t>141204776</t>
         </is>
       </c>
     </row>
@@ -3236,11 +3661,11 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Wagner Campos Silva</t>
+          <t>Caio Nunes Pinto</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -3249,17 +3674,22 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>628.169.480-56</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>473750890</t>
+          <t>908.001.770-10</t>
+        </is>
+      </c>
+      <c r="H86" t="inlineStr">
+        <is>
+          <t>435034240</t>
         </is>
       </c>
     </row>
@@ -3269,30 +3699,35 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Leonardo Gomes</t>
+          <t>Carolina Eduarda Melo</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>743.214.750-74</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>195429050</t>
+          <t>754.189.460-56</t>
+        </is>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>611221917</t>
         </is>
       </c>
     </row>
@@ -3302,30 +3737,35 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Gustavo Cavalcanti Lopes</t>
+          <t>Natália Martins Rodrigues Nascimento</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>923.935.850-10</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>165926559</t>
+          <t>244.570.930-09</t>
+        </is>
+      </c>
+      <c r="H88" t="inlineStr">
+        <is>
+          <t>815192692</t>
         </is>
       </c>
     </row>
@@ -3335,11 +3775,11 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Vanessa Pires Pinto</t>
+          <t>Larissa Gonçalves Mendes</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -3348,17 +3788,22 @@
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>404.861.590-43</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>430194903</t>
+          <t>683.994.450-61</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>405592816</t>
         </is>
       </c>
     </row>
@@ -3368,11 +3813,11 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Joaquim Almeida</t>
+          <t>Roberto Felipe Pires Lima</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -3386,12 +3831,17 @@
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>964.536.290-38</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>368181186</t>
+          <t>065.483.740-61</t>
+        </is>
+      </c>
+      <c r="H90" t="inlineStr">
+        <is>
+          <t>283882841</t>
         </is>
       </c>
     </row>
@@ -3401,11 +3851,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Marcelo Dias</t>
+          <t>Samuel Barros Moraes</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -3414,17 +3864,22 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>334.794.630-88</t>
+          <t>Superior completo</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>823345796</t>
+          <t>625.329.620-54</t>
+        </is>
+      </c>
+      <c r="H91" t="inlineStr">
+        <is>
+          <t>013135165</t>
         </is>
       </c>
     </row>
@@ -3434,11 +3889,11 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Paulo Ferreira</t>
+          <t>Guilherme Campos Melo</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -3447,17 +3902,22 @@
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>965.599.030-36</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>314244779</t>
+          <t>301.809.120-54</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>205164482</t>
         </is>
       </c>
     </row>
@@ -3467,30 +3927,35 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Ana Amanda Cardoso Fernandes</t>
+          <t>Gustavo Ferreira Ribeira</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>883.231.140-21</t>
+          <t>Superior incompleto</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>718139509</t>
+          <t>808.907.120-18</t>
+        </is>
+      </c>
+      <c r="H93" t="inlineStr">
+        <is>
+          <t>668103393</t>
         </is>
       </c>
     </row>
@@ -3500,30 +3965,35 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Rosana Gouveia Santos Moraes</t>
+          <t>Geraldo Santana Martins</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>953.671.250-42</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>625202866</t>
+          <t>088.070.930-81</t>
+        </is>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>524528662</t>
         </is>
       </c>
     </row>
@@ -3533,11 +4003,11 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Rafaela Alves Carvalho</t>
+          <t>Camila Ribeiro</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -3546,17 +4016,22 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>870.623.120-96</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>090422115</t>
+          <t>804.519.430-82</t>
+        </is>
+      </c>
+      <c r="H95" t="inlineStr">
+        <is>
+          <t>574471961</t>
         </is>
       </c>
     </row>
@@ -3566,11 +4041,11 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Isabela Pessoa Ramos</t>
+          <t>Carla Cardoso</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -3579,17 +4054,22 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>105.353.090-07</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>716483340</t>
+          <t>725.581.140-00</t>
+        </is>
+      </c>
+      <c r="H96" t="inlineStr">
+        <is>
+          <t>404465068</t>
         </is>
       </c>
     </row>
@@ -3599,30 +4079,35 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Alberto Nascimento Andrade</t>
+          <t>Cátia Tânia Nascimento Pires</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>077.368.520-06</t>
+          <t>Superior completo</t>
         </is>
       </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>398461322</t>
+          <t>687.837.170-80</t>
+        </is>
+      </c>
+      <c r="H97" t="inlineStr">
+        <is>
+          <t>906178100</t>
         </is>
       </c>
     </row>
@@ -3632,11 +4117,11 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Luciano Alberto Mendes Vieira</t>
+          <t>Anderson Nascimento Dias</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -3645,17 +4130,22 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>489.850.010-27</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>394514546</t>
+          <t>605.712.910-58</t>
+        </is>
+      </c>
+      <c r="H98" t="inlineStr">
+        <is>
+          <t>595416320</t>
         </is>
       </c>
     </row>
@@ -3665,30 +4155,35 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>João Campos</t>
+          <t>Patrícia Gouveia Andrade</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>600.279.900-10</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>420651346</t>
+          <t>338.842.120-01</t>
+        </is>
+      </c>
+      <c r="H99" t="inlineStr">
+        <is>
+          <t>490792353</t>
         </is>
       </c>
     </row>
@@ -3698,30 +4193,35 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Patrícia Karla Gomes Correia Gonçalves Dias</t>
+          <t>Felipe Sousa</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>427.720.200-45</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>027894756</t>
+          <t>279.421.300-88</t>
+        </is>
+      </c>
+      <c r="H100" t="inlineStr">
+        <is>
+          <t>138515614</t>
         </is>
       </c>
     </row>
@@ -3731,11 +4231,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Renato Nunes Andrade</t>
+          <t>Caio Carvalho Santana</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -3749,12 +4249,17 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>952.156.600-00</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>922158428</t>
+          <t>228.514.510-14</t>
+        </is>
+      </c>
+      <c r="H101" t="inlineStr">
+        <is>
+          <t>463736083</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização no gerador de nomes
</commit_message>
<xml_diff>
--- a/perfis_generated_openpyxl.xlsx
+++ b/perfis_generated_openpyxl.xlsx
@@ -474,11 +474,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Lucas Pedro Almeida Lima</t>
+          <t>André Álvaro Borges Machado</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -487,7 +487,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -502,12 +502,12 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>219.140.730-70</t>
+          <t>379.149.550-00</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>363456109</t>
+          <t>899076213</t>
         </is>
       </c>
     </row>
@@ -517,20 +517,20 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Gilberto Lima Fernandes</t>
+          <t>Natália Campos Ramos</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -545,12 +545,12 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>980.777.460-80</t>
+          <t>808.050.820-85</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>827797425</t>
+          <t>496664143</t>
         </is>
       </c>
     </row>
@@ -560,11 +560,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Simone Araújo Pereira</t>
+          <t>Carla Leticia Cardoso Nunes</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -573,7 +573,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -588,12 +588,12 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>372.009.970-99</t>
+          <t>031.286.110-92</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>748586035</t>
+          <t>415520384</t>
         </is>
       </c>
     </row>
@@ -603,11 +603,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Andréa Gouveia</t>
+          <t>Sueli Freitas Melo Pinto</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -616,7 +616,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -626,17 +626,17 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Desocupado</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>789.081.650-29</t>
+          <t>927.357.190-57</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>425375600</t>
+          <t>962299212</t>
         </is>
       </c>
     </row>
@@ -646,11 +646,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Eduardo Almeida Freitas</t>
+          <t>Paulo Silva Barbosa Ferreira</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -659,27 +659,27 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Fundamental incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Desocupado</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>981.708.410-89</t>
+          <t>906.200.340-09</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>083098079</t>
+          <t>037545016</t>
         </is>
       </c>
     </row>
@@ -689,20 +689,20 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Sueli Eduarda Moraes Pessoa</t>
+          <t>Diego Melo</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -712,17 +712,17 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
+          <t>Empregado: Setor privado (sem CLT)</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>303.231.290-64</t>
+          <t>096.369.690-43</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>631601001</t>
+          <t>229562224</t>
         </is>
       </c>
     </row>
@@ -732,11 +732,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Sueli Gouveia Ferreira</t>
+          <t>Ana Martins</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -745,27 +745,27 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Médio completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>855.268.730-56</t>
+          <t>448.575.560-65</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>053211279</t>
+          <t>478379477</t>
         </is>
       </c>
     </row>
@@ -775,40 +775,40 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Luiza Dias</t>
+          <t>Márcio José Freitas Andrade Almeida</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Médio completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Autonomo: Com CNPJ</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>753.131.320-08</t>
+          <t>602.685.150-00</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>059427547</t>
+          <t>955141308</t>
         </is>
       </c>
     </row>
@@ -818,11 +818,11 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Sebastião Pires</t>
+          <t>Joaquim Silva Silveira</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
@@ -831,27 +831,27 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Fundamental incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>369.761.980-24</t>
+          <t>282.227.320-05</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>645465045</t>
+          <t>018169698</t>
         </is>
       </c>
     </row>
@@ -861,11 +861,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Tatiana Gomes Ferreira Carvalho Nogueira</t>
+          <t>Patrícia Machado Melo</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -874,7 +874,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -889,12 +889,12 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>550.827.960-11</t>
+          <t>834.422.790-97</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>961523611</t>
+          <t>242228489</t>
         </is>
       </c>
     </row>
@@ -904,11 +904,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Isabela Carvalho Alves</t>
+          <t>Cecília Rocha Barros Carvalho</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -917,7 +917,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -927,17 +927,17 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>819.823.310-54</t>
+          <t>507.683.530-25</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>159444394</t>
+          <t>006508870</t>
         </is>
       </c>
     </row>
@@ -947,20 +947,20 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Jessica Nunes Araújo</t>
+          <t>Pedro Monteiro Cardoso</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -975,12 +975,12 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>138.398.750-56</t>
+          <t>133.688.450-98</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>346406513</t>
+          <t>840976251</t>
         </is>
       </c>
     </row>
@@ -990,11 +990,11 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Giovanni Santos Azevedo</t>
+          <t>Raul Santana</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
@@ -1003,7 +1003,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -1013,17 +1013,17 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Autonomo: Com CNPJ</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>254.357.570-70</t>
+          <t>888.100.640-54</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>909844276</t>
+          <t>267373026</t>
         </is>
       </c>
     </row>
@@ -1033,7 +1033,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>João Almeida Dias</t>
+          <t>Álvaro Pinto Rocha Moraes</t>
         </is>
       </c>
       <c r="C15" t="n">
@@ -1061,12 +1061,12 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>777.928.610-07</t>
+          <t>958.788.230-04</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>739875973</t>
+          <t>475580927</t>
         </is>
       </c>
     </row>
@@ -1076,11 +1076,11 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Patrícia Amanda Sousa Borges</t>
+          <t>Andréa Ferreira</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>39</v>
+        <v>5</v>
       </c>
       <c r="D16" t="inlineStr">
         <is>
@@ -1089,27 +1089,27 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Médio completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (sem CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>001.977.760-43</t>
+          <t>121.641.130-12</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>505089730</t>
+          <t>739758258</t>
         </is>
       </c>
     </row>
@@ -1119,11 +1119,11 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Wagner Alexandre Pires Cardoso</t>
+          <t>Armando Luciano Vieira</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D17" t="inlineStr">
         <is>
@@ -1132,7 +1132,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -1142,17 +1142,17 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>308.423.170-23</t>
+          <t>152.853.120-51</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>659293068</t>
+          <t>673658795</t>
         </is>
       </c>
     </row>
@@ -1162,20 +1162,20 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Larissa Ferreira Costa</t>
+          <t>Vicente André Nascimento Sousa</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -1190,12 +1190,12 @@
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>989.246.480-04</t>
+          <t>395.386.700-86</t>
         </is>
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>112869303</t>
+          <t>273786816</t>
         </is>
       </c>
     </row>
@@ -1205,11 +1205,11 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Vitor Correia Almeida</t>
+          <t>Diego Ribeiro</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D19" t="inlineStr">
         <is>
@@ -1218,27 +1218,27 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Superior incompleto</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>Empregado: Setor ublico (estatutário ou militar)</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>571.554.670-22</t>
+          <t>297.917.360-65</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>230750077</t>
+          <t>471561993</t>
         </is>
       </c>
     </row>
@@ -1248,11 +1248,11 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Pedro Gomes Sousa</t>
+          <t>César Gomes</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D20" t="inlineStr">
         <is>
@@ -1271,17 +1271,17 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>982.520.280-71</t>
+          <t>160.003.510-89</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>618126717</t>
+          <t>970140836</t>
         </is>
       </c>
     </row>
@@ -1291,40 +1291,40 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Marcelo Alexandre Gonçalves</t>
+          <t>Jessica Freitas Cardoso</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Empregado: Setor ublico (estatutário ou militar)</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>841.944.980-62</t>
+          <t>953.236.160-08</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>785117599</t>
+          <t>782780354</t>
         </is>
       </c>
     </row>
@@ -1334,11 +1334,11 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Amanda Renata Cardoso Costa Azevedo Carvalho</t>
+          <t>Jéssica Gouveia Pinto</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -1352,22 +1352,22 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Superior incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>569.228.550-94</t>
+          <t>498.570.490-36</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>265494545</t>
+          <t>929104625</t>
         </is>
       </c>
     </row>
@@ -1377,20 +1377,20 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Alberto André Barros</t>
+          <t>Mariana Oliveira Gomes</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -1400,17 +1400,17 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>Autonomo: Com CNPJ</t>
+          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>593.444.870-65</t>
+          <t>768.884.210-74</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>145289180</t>
+          <t>409821590</t>
         </is>
       </c>
     </row>
@@ -1420,11 +1420,11 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Sebastião Rocha Gonçalves</t>
+          <t>Raul Vieira Rodrigues</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
@@ -1448,12 +1448,12 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>695.360.610-07</t>
+          <t>911.418.020-07</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>044826750</t>
+          <t>315442995</t>
         </is>
       </c>
     </row>
@@ -1463,11 +1463,11 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Renata Cavalcanti</t>
+          <t>Fernanda Valéria Oliveira Dias</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="D25" t="inlineStr">
         <is>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -1486,17 +1486,17 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Empregado: Setor privado (sem CLT)</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>259.980.540-67</t>
+          <t>669.100.700-03</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>750881263</t>
+          <t>148612271</t>
         </is>
       </c>
     </row>
@@ -1506,11 +1506,11 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Mariana Pires</t>
+          <t>Andréa Cecília Pereira Azevedo</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>51</v>
+        <v>21</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
@@ -1519,12 +1519,12 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Preta</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Médio completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1534,12 +1534,12 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>733.695.060-41</t>
+          <t>354.985.460-92</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>161240609</t>
+          <t>130453484</t>
         </is>
       </c>
     </row>
@@ -1549,20 +1549,20 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Tânia Eduarda Borges Rodrigues</t>
+          <t>Alberto César Barros</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1572,17 +1572,17 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>Empregado: Setor ublico (estatutário ou militar)</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>054.137.180-04</t>
+          <t>172.597.890-34</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>010570380</t>
+          <t>434716875</t>
         </is>
       </c>
     </row>
@@ -1592,11 +1592,11 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Larissa Lima</t>
+          <t>Regina Pereira Gomes</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
@@ -1620,12 +1620,12 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>841.532.130-98</t>
+          <t>343.993.120-09</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>685575204</t>
+          <t>277445157</t>
         </is>
       </c>
     </row>
@@ -1635,11 +1635,11 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Felipe Rocha</t>
+          <t>Wagner Arnaldo Silva</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="D29" t="inlineStr">
         <is>
@@ -1658,17 +1658,17 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (sem CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>323.391.450-40</t>
+          <t>744.984.570-99</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>271021707</t>
+          <t>060812675</t>
         </is>
       </c>
     </row>
@@ -1678,40 +1678,40 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Raul Dias Freitas</t>
+          <t>Carla Mendes Andrade</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Médio completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Desocupado</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>003.874.760-08</t>
+          <t>480.478.580-92</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>332660665</t>
+          <t>436330737</t>
         </is>
       </c>
     </row>
@@ -1721,11 +1721,11 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Luis Ribeira Nunes</t>
+          <t>Sebastião Rodrigues Andrade</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
@@ -1739,22 +1739,22 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>Desocupado</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>740.802.750-56</t>
+          <t>027.648.950-03</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>559309347</t>
+          <t>784204161</t>
         </is>
       </c>
     </row>
@@ -1764,20 +1764,20 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Lucas Ribeiro</t>
+          <t>Tatiane Carvalho Martins</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -1787,17 +1787,17 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>Empregado: Setor publico (sem CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>511.239.770-54</t>
+          <t>862.961.010-74</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>620298058</t>
+          <t>246861047</t>
         </is>
       </c>
     </row>
@@ -1807,20 +1807,20 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Samuel Lopes Ribeira</t>
+          <t>Carolina Nogueira</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>21</v>
+        <v>2</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -1830,17 +1830,17 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>116.320.810-83</t>
+          <t>092.105.500-56</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>269364296</t>
+          <t>418793630</t>
         </is>
       </c>
     </row>
@@ -1850,40 +1850,40 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Diego Vitor Ferreira Gomes</t>
+          <t>Leticia Santana Oliveira</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Superior incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>Autonomo: Com CNPJ</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>065.887.450-01</t>
+          <t>759.354.970-42</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>878287805</t>
+          <t>575477198</t>
         </is>
       </c>
     </row>
@@ -1893,11 +1893,11 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>João Roberto Gonçalves Vieira Almeida</t>
+          <t>Paulo Cavalcanti</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>20</v>
+        <v>47</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
@@ -1911,22 +1911,22 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Autonomo: Com CNPJ</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>214.637.400-42</t>
+          <t>727.495.540-39</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>225878513</t>
+          <t>717909630</t>
         </is>
       </c>
     </row>
@@ -1936,11 +1936,11 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Tatiana Mariana Costa</t>
+          <t>Laura Nunes</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
@@ -1949,7 +1949,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -1959,17 +1959,17 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>132.228.160-26</t>
+          <t>345.609.850-22</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>560943836</t>
+          <t>826002443</t>
         </is>
       </c>
     </row>
@@ -1979,11 +1979,11 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Fernando Renato Andrade Lima Fernandes</t>
+          <t>Ricardo Araújo Machado Pessoa Campos</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
@@ -1992,7 +1992,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -2002,17 +2002,17 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (sem CLT)</t>
+          <t>Autonomo: Com CNPJ</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>083.512.850-48</t>
+          <t>275.263.820-54</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>459623603</t>
+          <t>339752098</t>
         </is>
       </c>
     </row>
@@ -2022,11 +2022,11 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Sandra Amanda Ferreira Ribeiro Ramos Vieira</t>
+          <t>Rafaela Ribeira Pires Correia Monteiro</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
@@ -2035,7 +2035,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -2050,12 +2050,12 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>496.315.960-01</t>
+          <t>942.081.950-70</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>821214710</t>
+          <t>186515988</t>
         </is>
       </c>
     </row>
@@ -2065,11 +2065,11 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Sebastião Pires</t>
+          <t>Geraldo Costa Santana</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
@@ -2088,17 +2088,17 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Desocupado</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>034.225.260-72</t>
+          <t>361.011.190-92</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>358300336</t>
+          <t>738443551</t>
         </is>
       </c>
     </row>
@@ -2108,20 +2108,20 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Isaac Felipe Freitas</t>
+          <t>Márcia Cardoso Araújo</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -2136,12 +2136,12 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>969.585.990-98</t>
+          <t>298.857.790-00</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>122713199</t>
+          <t>780549306</t>
         </is>
       </c>
     </row>
@@ -2151,11 +2151,11 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Regina Nascimento Gomes Lima Monteiro</t>
+          <t>Rafaela Helena Silveira Nogueira</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>47</v>
+        <v>24</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
@@ -2164,27 +2164,27 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Superior completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>018.789.720-49</t>
+          <t>931.253.590-07</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>196574091</t>
+          <t>936384540</t>
         </is>
       </c>
     </row>
@@ -2194,11 +2194,11 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Larissa Pinto Nogueira</t>
+          <t>Bianca Moraes</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
@@ -2207,7 +2207,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -2217,17 +2217,17 @@
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (sem CLT)</t>
+          <t>Empregado: Setor publico (sem CLT)</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>737.465.400-62</t>
+          <t>938.057.620-03</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>249920159</t>
+          <t>386567500</t>
         </is>
       </c>
     </row>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Carlos Lopes</t>
+          <t>Thais Cavalcanti Nunes</t>
         </is>
       </c>
       <c r="C43" t="n">
@@ -2245,12 +2245,12 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2260,17 +2260,17 @@
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>Desocupado</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>280.356.550-19</t>
+          <t>493.754.310-53</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
         <is>
-          <t>181460235</t>
+          <t>841904739</t>
         </is>
       </c>
     </row>
@@ -2280,11 +2280,11 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Flávia Lima Ramos Castro</t>
+          <t>Valéria Mendes Andrade</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
@@ -2293,12 +2293,12 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Fundamental incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -2308,12 +2308,12 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>174.294.320-93</t>
+          <t>659.370.870-46</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>961347647</t>
+          <t>234110135</t>
         </is>
       </c>
     </row>
@@ -2323,40 +2323,40 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Márcio Ribeiro Campos</t>
+          <t>Thais Ramos Mendes</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>930.260.160-98</t>
+          <t>961.820.910-53</t>
         </is>
       </c>
       <c r="I45" t="inlineStr">
         <is>
-          <t>364570390</t>
+          <t>022657408</t>
         </is>
       </c>
     </row>
@@ -2366,11 +2366,11 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Álvaro Silveira Cardoso</t>
+          <t>Thiago Moraes</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
@@ -2389,17 +2389,17 @@
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>767.112.810-47</t>
+          <t>191.478.130-91</t>
         </is>
       </c>
       <c r="I46" t="inlineStr">
         <is>
-          <t>158038782</t>
+          <t>055467665</t>
         </is>
       </c>
     </row>
@@ -2409,20 +2409,20 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Vanessa Vieira Lopes Correia</t>
+          <t>Vicente Pereira Dias</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
@@ -2437,12 +2437,12 @@
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>681.151.560-00</t>
+          <t>515.404.180-14</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
         <is>
-          <t>576974858</t>
+          <t>925164330</t>
         </is>
       </c>
     </row>
@@ -2452,40 +2452,40 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Tatiane Borges Pereira</t>
+          <t>Geraldo Silveira Castro</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Superior completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>Empregador: Com CNPJ</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H48" t="inlineStr">
         <is>
-          <t>219.600.850-85</t>
+          <t>926.614.780-00</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
         <is>
-          <t>528797425</t>
+          <t>070649358</t>
         </is>
       </c>
     </row>
@@ -2495,40 +2495,40 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Elias Thiago Mendes Pereira Fernandes</t>
+          <t>Tatiana Machado Rocha Gouveia Carvalho</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Autonomo: Com CNPJ</t>
         </is>
       </c>
       <c r="H49" t="inlineStr">
         <is>
-          <t>976.090.480-20</t>
+          <t>577.868.200-00</t>
         </is>
       </c>
       <c r="I49" t="inlineStr">
         <is>
-          <t>671201755</t>
+          <t>051754010</t>
         </is>
       </c>
     </row>
@@ -2538,20 +2538,20 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Mariana Eduarda Machado</t>
+          <t>Arnaldo Fernando Moraes Costa</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
@@ -2561,17 +2561,17 @@
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>Empregado: Setor publico (sem CLT)</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>866.159.360-38</t>
+          <t>339.009.090-83</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
         <is>
-          <t>969355076</t>
+          <t>753025452</t>
         </is>
       </c>
     </row>
@@ -2581,25 +2581,25 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Fernanda Nascimento Costa Nascimento</t>
+          <t>Diego Carvalho Martins Gomes</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Fundamental incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2609,12 +2609,12 @@
       </c>
       <c r="H51" t="inlineStr">
         <is>
-          <t>267.952.250-89</t>
+          <t>198.960.500-15</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
         <is>
-          <t>082371233</t>
+          <t>241472106</t>
         </is>
       </c>
     </row>
@@ -2624,40 +2624,40 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Lorena Lima Gonçalves</t>
+          <t>Marcelo Ribeiro Carvalho</t>
         </is>
       </c>
       <c r="C52" t="n">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Superior completo</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>Empregado: Setor publico (sem CLT)</t>
+          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
         </is>
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>095.508.180-71</t>
+          <t>490.376.480-02</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
         <is>
-          <t>924950728</t>
+          <t>374038627</t>
         </is>
       </c>
     </row>
@@ -2667,11 +2667,11 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Gustavo Lopes Pires</t>
+          <t>Vinícius Luciano Borges</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="D53" t="inlineStr">
         <is>
@@ -2680,27 +2680,27 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>551.115.070-35</t>
+          <t>059.443.260-00</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
         <is>
-          <t>258152986</t>
+          <t>209310123</t>
         </is>
       </c>
     </row>
@@ -2710,20 +2710,20 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Sandra Gonçalves Machado Pereira</t>
+          <t>Sebastião Costa Monteiro Barros Pires</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
@@ -2733,17 +2733,17 @@
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>Empregador: Sem CNPJ</t>
+          <t>Autonomo: Com CNPJ</t>
         </is>
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>777.469.990-26</t>
+          <t>627.079.590-73</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
         <is>
-          <t>899254670</t>
+          <t>667980440</t>
         </is>
       </c>
     </row>
@@ -2753,20 +2753,20 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Aline Ferreira Mendes</t>
+          <t>César Correia Lima Ribeiro</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F55" t="inlineStr">
@@ -2781,12 +2781,12 @@
       </c>
       <c r="H55" t="inlineStr">
         <is>
-          <t>773.992.430-00</t>
+          <t>050.299.500-95</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
         <is>
-          <t>461486777</t>
+          <t>270023541</t>
         </is>
       </c>
     </row>
@@ -2796,20 +2796,20 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Alberto Alves Freitas Vieira</t>
+          <t>Tânia Lopes Almeida</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
@@ -2824,12 +2824,12 @@
       </c>
       <c r="H56" t="inlineStr">
         <is>
-          <t>067.575.750-94</t>
+          <t>564.691.900-22</t>
         </is>
       </c>
       <c r="I56" t="inlineStr">
         <is>
-          <t>000658490</t>
+          <t>520192260</t>
         </is>
       </c>
     </row>
@@ -2839,11 +2839,11 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Ronaldo Moraes Campos</t>
+          <t>Hugo Diego Monteiro</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -2852,27 +2852,27 @@
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Fundamental incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Empregado: Setor privado (sem CLT)</t>
         </is>
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>654.081.740-18</t>
+          <t>798.712.880-50</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
         <is>
-          <t>496238745</t>
+          <t>563867863</t>
         </is>
       </c>
     </row>
@@ -2882,40 +2882,40 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Rosana Sueli Pires Ferreira Borges</t>
+          <t>Thiago Melo Borges Castro Nunes</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Sem instrução</t>
         </is>
       </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Autonomo: Com CNPJ</t>
         </is>
       </c>
       <c r="H58" t="inlineStr">
         <is>
-          <t>920.050.700-09</t>
+          <t>905.979.660-87</t>
         </is>
       </c>
       <c r="I58" t="inlineStr">
         <is>
-          <t>215465085</t>
+          <t>660702843</t>
         </is>
       </c>
     </row>
@@ -2925,40 +2925,40 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Hugo Almeida Oliveira</t>
+          <t>Cecília Melo Lopes</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Fundamental incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>Empregado: Setor publico (CLT)</t>
+          <t>Empregado: Setor privado (sem CLT)</t>
         </is>
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>971.820.350-81</t>
+          <t>624.478.800-14</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
         <is>
-          <t>946988119</t>
+          <t>972714817</t>
         </is>
       </c>
     </row>
@@ -2968,20 +2968,20 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Natália Leticia Fernandes</t>
+          <t>Arnaldo Lima Pereira</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
@@ -2991,17 +2991,17 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Empregado: Setor privado (sem CLT)</t>
         </is>
       </c>
       <c r="H60" t="inlineStr">
         <is>
-          <t>863.764.180-66</t>
+          <t>252.190.070-25</t>
         </is>
       </c>
       <c r="I60" t="inlineStr">
         <is>
-          <t>139938211</t>
+          <t>107517713</t>
         </is>
       </c>
     </row>
@@ -3011,11 +3011,11 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Álvaro Antônio Santos Sousa</t>
+          <t>Caio Nascimento Santana Lopes</t>
         </is>
       </c>
       <c r="C61" t="n">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -3024,27 +3024,27 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Empregado: Setor publico (sem CLT)</t>
         </is>
       </c>
       <c r="H61" t="inlineStr">
         <is>
-          <t>530.964.920-42</t>
+          <t>372.342.850-91</t>
         </is>
       </c>
       <c r="I61" t="inlineStr">
         <is>
-          <t>612693365</t>
+          <t>256368437</t>
         </is>
       </c>
     </row>
@@ -3054,11 +3054,11 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Camila Tatiane Martins Pereira</t>
+          <t>Thais Tânia Barros Correia</t>
         </is>
       </c>
       <c r="C62" t="n">
-        <v>41</v>
+        <v>11</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -3067,27 +3067,27 @@
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Médio completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (sem CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H62" t="inlineStr">
         <is>
-          <t>238.768.950-06</t>
+          <t>840.286.140-74</t>
         </is>
       </c>
       <c r="I62" t="inlineStr">
         <is>
-          <t>414806863</t>
+          <t>571068179</t>
         </is>
       </c>
     </row>
@@ -3097,40 +3097,40 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Sueli Pinto Barbosa</t>
+          <t>Álvaro Ribeira Martins</t>
         </is>
       </c>
       <c r="C63" t="n">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Médio completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>234.318.700-23</t>
+          <t>729.209.880-00</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>673734759</t>
+          <t>620056140</t>
         </is>
       </c>
     </row>
@@ -3140,11 +3140,11 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Renata Lima Freitas Melo</t>
+          <t>Sandra Camila Pessoa Santos</t>
         </is>
       </c>
       <c r="C64" t="n">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -3153,7 +3153,7 @@
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F64" t="inlineStr">
@@ -3163,17 +3163,17 @@
       </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>Empregado: Setor publico (sem CLT)</t>
+          <t>Desocupado</t>
         </is>
       </c>
       <c r="H64" t="inlineStr">
         <is>
-          <t>357.770.950-20</t>
+          <t>675.244.200-21</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
         <is>
-          <t>727345668</t>
+          <t>684738157</t>
         </is>
       </c>
     </row>
@@ -3183,11 +3183,11 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Larissa Priscila Barros</t>
+          <t>Natália Juliana Silveira Campos</t>
         </is>
       </c>
       <c r="C65" t="n">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -3196,7 +3196,7 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
@@ -3206,17 +3206,17 @@
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Empregador: Com CNPJ</t>
         </is>
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>296.821.070-08</t>
+          <t>561.990.160-25</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
         <is>
-          <t>210723553</t>
+          <t>084901075</t>
         </is>
       </c>
     </row>
@@ -3226,11 +3226,11 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Roberta Oliveira Fernandes</t>
+          <t>Isabela Alves Carvalho</t>
         </is>
       </c>
       <c r="C66" t="n">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -3254,12 +3254,12 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>391.365.150-00</t>
+          <t>393.878.760-04</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
         <is>
-          <t>750656715</t>
+          <t>741168738</t>
         </is>
       </c>
     </row>
@@ -3269,11 +3269,11 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Raul Leonardo Almeida</t>
+          <t>Ronaldo Pereira</t>
         </is>
       </c>
       <c r="C67" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -3282,7 +3282,7 @@
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F67" t="inlineStr">
@@ -3292,17 +3292,17 @@
       </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Empregado: Setor privado (sem CLT)</t>
         </is>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>372.906.620-08</t>
+          <t>993.282.990-04</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
         <is>
-          <t>956570082</t>
+          <t>468401128</t>
         </is>
       </c>
     </row>
@@ -3312,11 +3312,11 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Fernanda Cavalcanti Sousa Pereira</t>
+          <t>Valéria Silveira</t>
         </is>
       </c>
       <c r="C68" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -3340,12 +3340,12 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>034.270.810-44</t>
+          <t>201.022.320-91</t>
         </is>
       </c>
       <c r="I68" t="inlineStr">
         <is>
-          <t>961101250</t>
+          <t>977251878</t>
         </is>
       </c>
     </row>
@@ -3355,11 +3355,11 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Andréa Andrade Ferreira</t>
+          <t>Rosana Pinto</t>
         </is>
       </c>
       <c r="C69" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -3368,27 +3368,27 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Sem instrução</t>
+          <t>Superior completo</t>
         </is>
       </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>Empregado: Trabalhador doméstico (CLT)</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>538.706.530-43</t>
+          <t>519.021.320-09</t>
         </is>
       </c>
       <c r="I69" t="inlineStr">
         <is>
-          <t>693872205</t>
+          <t>008864460</t>
         </is>
       </c>
     </row>
@@ -3398,11 +3398,11 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Renata Márcia Correia Gonçalves</t>
+          <t>Rosana Pinto</t>
         </is>
       </c>
       <c r="C70" t="n">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -3421,17 +3421,17 @@
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H70" t="inlineStr">
         <is>
-          <t>423.880.560-71</t>
+          <t>390.426.510-59</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
         <is>
-          <t>594668650</t>
+          <t>287861524</t>
         </is>
       </c>
     </row>
@@ -3441,20 +3441,20 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Cecília Costa</t>
+          <t>Caio Rodrigues Nunes</t>
         </is>
       </c>
       <c r="C71" t="n">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F71" t="inlineStr">
@@ -3469,12 +3469,12 @@
       </c>
       <c r="H71" t="inlineStr">
         <is>
-          <t>564.230.990-06</t>
+          <t>948.511.600-46</t>
         </is>
       </c>
       <c r="I71" t="inlineStr">
         <is>
-          <t>198544990</t>
+          <t>299173910</t>
         </is>
       </c>
     </row>
@@ -3484,7 +3484,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Rosana Santos Gonçalves</t>
+          <t>José Silveira Correia</t>
         </is>
       </c>
       <c r="C72" t="n">
@@ -3492,12 +3492,12 @@
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
@@ -3512,12 +3512,12 @@
       </c>
       <c r="H72" t="inlineStr">
         <is>
-          <t>495.700.930-99</t>
+          <t>663.249.130-82</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
         <is>
-          <t>542163076</t>
+          <t>135150530</t>
         </is>
       </c>
     </row>
@@ -3527,40 +3527,40 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Sérgio Thiago Silva Vieira</t>
+          <t>Renata Cátia Moraes</t>
         </is>
       </c>
       <c r="C73" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Superior completo</t>
         </is>
       </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H73" t="inlineStr">
         <is>
-          <t>355.913.810-81</t>
+          <t>437.226.710-00</t>
         </is>
       </c>
       <c r="I73" t="inlineStr">
         <is>
-          <t>401236395</t>
+          <t>935793096</t>
         </is>
       </c>
     </row>
@@ -3570,20 +3570,20 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Sérgio Elias Ribeiro</t>
+          <t>Fábio Pessoa Machado</t>
         </is>
       </c>
       <c r="C74" t="n">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Não-Binário</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Preto(a)</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
@@ -3593,17 +3593,17 @@
       </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
         </is>
       </c>
       <c r="H74" t="inlineStr">
         <is>
-          <t>789.997.680-40</t>
+          <t>259.801.070-10</t>
         </is>
       </c>
       <c r="I74" t="inlineStr">
         <is>
-          <t>790236676</t>
+          <t>515307234</t>
         </is>
       </c>
     </row>
@@ -3613,40 +3613,40 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Leonardo Correia</t>
+          <t>Flávia Gonçalves Borges Santos</t>
         </is>
       </c>
       <c r="C75" t="n">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H75" t="inlineStr">
         <is>
-          <t>240.847.960-69</t>
+          <t>498.094.190-74</t>
         </is>
       </c>
       <c r="I75" t="inlineStr">
         <is>
-          <t>238104368</t>
+          <t>805018782</t>
         </is>
       </c>
     </row>
@@ -3656,11 +3656,11 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Maria Costa</t>
+          <t>Ana Ribeira Martins</t>
         </is>
       </c>
       <c r="C76" t="n">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -3669,27 +3669,27 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (sem CLT)</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H76" t="inlineStr">
         <is>
-          <t>792.738.430-93</t>
+          <t>826.645.100-10</t>
         </is>
       </c>
       <c r="I76" t="inlineStr">
         <is>
-          <t>398134491</t>
+          <t>605025690</t>
         </is>
       </c>
     </row>
@@ -3699,40 +3699,40 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Cecília Machado</t>
+          <t>Gilberto Alves Gomes</t>
         </is>
       </c>
       <c r="C77" t="n">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Superior completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Empregado: Setor publico (sem CLT)</t>
         </is>
       </c>
       <c r="H77" t="inlineStr">
         <is>
-          <t>154.323.410-00</t>
+          <t>442.532.230-44</t>
         </is>
       </c>
       <c r="I77" t="inlineStr">
         <is>
-          <t>597293592</t>
+          <t>069921284</t>
         </is>
       </c>
     </row>
@@ -3742,40 +3742,40 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Marcelo César Pinto Melo</t>
+          <t>Márcia Nascimento Gouveia</t>
         </is>
       </c>
       <c r="C78" t="n">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Fundamental incompleto</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H78" t="inlineStr">
         <is>
-          <t>036.554.070-68</t>
+          <t>375.124.390-91</t>
         </is>
       </c>
       <c r="I78" t="inlineStr">
         <is>
-          <t>562319038</t>
+          <t>749162000</t>
         </is>
       </c>
     </row>
@@ -3785,20 +3785,20 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Karla Pires Carvalho Nogueira</t>
+          <t>Rafael Gomes Nogueira Pires Costa</t>
         </is>
       </c>
       <c r="C79" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F79" t="inlineStr">
@@ -3813,12 +3813,12 @@
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>914.276.090-98</t>
+          <t>258.686.400-04</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>328749713</t>
+          <t>372217026</t>
         </is>
       </c>
     </row>
@@ -3828,11 +3828,11 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Gustavo Cavalcanti Dias</t>
+          <t>Sergio Ribeira</t>
         </is>
       </c>
       <c r="C80" t="n">
-        <v>23</v>
+        <v>0</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -3841,7 +3841,7 @@
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
@@ -3851,17 +3851,17 @@
       </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>Desocupado</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>193.705.380-62</t>
+          <t>340.789.770-73</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
         <is>
-          <t>182867885</t>
+          <t>073179878</t>
         </is>
       </c>
     </row>
@@ -3871,11 +3871,11 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>João Geraldo Martins Gomes</t>
+          <t>José Machado Ribeira</t>
         </is>
       </c>
       <c r="C81" t="n">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -3889,22 +3889,22 @@
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Médio completo</t>
+          <t>Médio incompleto</t>
         </is>
       </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (sem CLT)</t>
+          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
         </is>
       </c>
       <c r="H81" t="inlineStr">
         <is>
-          <t>738.739.870-40</t>
+          <t>760.172.510-31</t>
         </is>
       </c>
       <c r="I81" t="inlineStr">
         <is>
-          <t>817545073</t>
+          <t>192836436</t>
         </is>
       </c>
     </row>
@@ -3914,11 +3914,11 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Luiza Ramos Ferreira Machado</t>
+          <t>Thais Alves Almeida</t>
         </is>
       </c>
       <c r="C82" t="n">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -3927,7 +3927,7 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
@@ -3937,17 +3937,17 @@
       </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (sem CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H82" t="inlineStr">
         <is>
-          <t>432.366.690-04</t>
+          <t>087.576.480-00</t>
         </is>
       </c>
       <c r="I82" t="inlineStr">
         <is>
-          <t>620215030</t>
+          <t>842239744</t>
         </is>
       </c>
     </row>
@@ -3957,20 +3957,20 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Bianca Melo Pinto</t>
+          <t>César Mendes Barros</t>
         </is>
       </c>
       <c r="C83" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
@@ -3980,17 +3980,17 @@
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>164.472.010-80</t>
+          <t>037.229.040-05</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>268636380</t>
+          <t>756683391</t>
         </is>
       </c>
     </row>
@@ -4000,11 +4000,11 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Ronaldo Sousa</t>
+          <t>Sebastião Wagner Nascimento Melo</t>
         </is>
       </c>
       <c r="C84" t="n">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -4018,7 +4018,7 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Médio completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G84" t="inlineStr">
@@ -4028,12 +4028,12 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>575.245.310-01</t>
+          <t>295.482.700-99</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
         <is>
-          <t>087099189</t>
+          <t>789859936</t>
         </is>
       </c>
     </row>
@@ -4043,20 +4043,20 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Luis Carvalho Pires Lopes</t>
+          <t>Valéria Fernandes Pires</t>
         </is>
       </c>
       <c r="C85" t="n">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
@@ -4066,17 +4066,17 @@
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>453.886.630-00</t>
+          <t>906.153.570-08</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>786113251</t>
+          <t>005162013</t>
         </is>
       </c>
     </row>
@@ -4086,20 +4086,20 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Carlos Machado</t>
+          <t>Ana Silva</t>
         </is>
       </c>
       <c r="C86" t="n">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
@@ -4109,17 +4109,17 @@
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>504.133.330-00</t>
+          <t>072.999.060-58</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
         <is>
-          <t>898745911</t>
+          <t>476129806</t>
         </is>
       </c>
     </row>
@@ -4129,25 +4129,25 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Raul Gilberto Lopes Ferreira</t>
+          <t>Tânia Santos</t>
         </is>
       </c>
       <c r="C87" t="n">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Médio completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G87" t="inlineStr">
@@ -4157,12 +4157,12 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>364.229.210-04</t>
+          <t>637.173.350-81</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>119475179</t>
+          <t>767116136</t>
         </is>
       </c>
     </row>
@@ -4172,20 +4172,20 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Wagner Correia Santana</t>
+          <t>Vanessa Sousa Pereira</t>
         </is>
       </c>
       <c r="C88" t="n">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
@@ -4195,17 +4195,17 @@
       </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>923.572.670-03</t>
+          <t>396.195.220-52</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
         <is>
-          <t>303845337</t>
+          <t>534701995</t>
         </is>
       </c>
     </row>
@@ -4215,40 +4215,40 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Ronaldo Machado Campos</t>
+          <t>Bianca Camila Rodrigues</t>
         </is>
       </c>
       <c r="C89" t="n">
-        <v>7</v>
+        <v>36</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E89" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Superior completo</t>
         </is>
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Empregado: Setor publico (CLT)</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
         <is>
-          <t>910.004.190-45</t>
+          <t>136.980.780-58</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
         <is>
-          <t>488475470</t>
+          <t>160303227</t>
         </is>
       </c>
     </row>
@@ -4258,20 +4258,20 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>André Pires</t>
+          <t>Amanda Gomes</t>
         </is>
       </c>
       <c r="C90" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
@@ -4286,12 +4286,12 @@
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>388.631.340-90</t>
+          <t>300.948.770-33</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>533907273</t>
+          <t>540787123</t>
         </is>
       </c>
     </row>
@@ -4301,11 +4301,11 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>Amanda Costa Cardoso Gomes</t>
+          <t>Aline Borges Rocha</t>
         </is>
       </c>
       <c r="C91" t="n">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -4314,27 +4314,27 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Superior completo</t>
+          <t>Médio incompleto</t>
         </is>
       </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>Empregador: Com CNPJ</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="H91" t="inlineStr">
         <is>
-          <t>799.103.490-94</t>
+          <t>801.182.140-71</t>
         </is>
       </c>
       <c r="I91" t="inlineStr">
         <is>
-          <t>458608712</t>
+          <t>090456911</t>
         </is>
       </c>
     </row>
@@ -4344,40 +4344,40 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Luiza Gomes Cavalcanti</t>
+          <t>Sebastião Alves Ferreira</t>
         </is>
       </c>
       <c r="C92" t="n">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Não-Binário</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branco(a)</t>
         </is>
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Médio completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>Empregado: Setor publico (sem CLT)</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="H92" t="inlineStr">
         <is>
-          <t>632.394.260-72</t>
+          <t>797.649.710-32</t>
         </is>
       </c>
       <c r="I92" t="inlineStr">
         <is>
-          <t>554504343</t>
+          <t>017523553</t>
         </is>
       </c>
     </row>
@@ -4387,11 +4387,11 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Alexandre Andrade Campos</t>
+          <t>Alberto Silva Mendes</t>
         </is>
       </c>
       <c r="C93" t="n">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -4405,22 +4405,22 @@
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Fundamental completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (sem CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H93" t="inlineStr">
         <is>
-          <t>444.304.810-32</t>
+          <t>755.249.600-24</t>
         </is>
       </c>
       <c r="I93" t="inlineStr">
         <is>
-          <t>247693190</t>
+          <t>087592787</t>
         </is>
       </c>
     </row>
@@ -4430,11 +4430,11 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Marcelo Sousa Pereira</t>
+          <t>Raul Freitas</t>
         </is>
       </c>
       <c r="C94" t="n">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -4443,7 +4443,7 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
@@ -4453,17 +4453,17 @@
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Empregado: Setor publico (sem CLT)</t>
         </is>
       </c>
       <c r="H94" t="inlineStr">
         <is>
-          <t>682.170.010-90</t>
+          <t>304.821.440-25</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
         <is>
-          <t>690693389</t>
+          <t>453292712</t>
         </is>
       </c>
     </row>
@@ -4473,20 +4473,20 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Fernanda Monteiro</t>
+          <t>Ricardo Pessoa Melo</t>
         </is>
       </c>
       <c r="C95" t="n">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
@@ -4496,17 +4496,17 @@
       </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>951.568.530-30</t>
+          <t>317.636.000-25</t>
         </is>
       </c>
       <c r="I95" t="inlineStr">
         <is>
-          <t>476888109</t>
+          <t>493549132</t>
         </is>
       </c>
     </row>
@@ -4516,40 +4516,40 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Anderson Campos Cavalcanti Monteiro</t>
+          <t>Carolina Melo Silva</t>
         </is>
       </c>
       <c r="C96" t="n">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Superior completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>Autonomo: Com CNPJ</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>766.230.730-19</t>
+          <t>148.937.220-26</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>887824542</t>
+          <t>342925770</t>
         </is>
       </c>
     </row>
@@ -4559,20 +4559,20 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Tatiana Castro Gonçalves</t>
+          <t>César Santos Araújo Rodrigues Carvalho</t>
         </is>
       </c>
       <c r="C97" t="n">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
@@ -4587,12 +4587,12 @@
       </c>
       <c r="H97" t="inlineStr">
         <is>
-          <t>496.946.730-70</t>
+          <t>517.773.020-48</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
         <is>
-          <t>949376522</t>
+          <t>024452989</t>
         </is>
       </c>
     </row>
@@ -4602,40 +4602,40 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Eduardo Silva</t>
+          <t>Sandra Brenda Sousa Lima</t>
         </is>
       </c>
       <c r="C98" t="n">
-        <v>47</v>
+        <v>21</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
-          <t>Não-Binário</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Pardo(a)</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Fundamental incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>341.278.850-33</t>
+          <t>065.489.790-52</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>015832106</t>
+          <t>481861804</t>
         </is>
       </c>
     </row>
@@ -4645,40 +4645,40 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Paulo Gouveia</t>
+          <t>Sandra Priscila Ribeiro Fernandes</t>
         </is>
       </c>
       <c r="C99" t="n">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>Empregado: Setor publico (sem CLT)</t>
+          <t>Empregado: Setor privado (sem CLT)</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>056.107.670-75</t>
+          <t>712.441.910-78</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>571447695</t>
+          <t>509216577</t>
         </is>
       </c>
     </row>
@@ -4688,11 +4688,11 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Natália Priscila Sousa Nunes Gomes</t>
+          <t>Mônica Gomes Dias</t>
         </is>
       </c>
       <c r="C100" t="n">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -4711,17 +4711,17 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>Empregado: Setor ublico (estatutário ou militar)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>276.390.290-15</t>
+          <t>868.958.560-56</t>
         </is>
       </c>
       <c r="I100" t="inlineStr">
         <is>
-          <t>000652586</t>
+          <t>214094481</t>
         </is>
       </c>
     </row>
@@ -4731,11 +4731,11 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Brenda Barros Costa</t>
+          <t>Andressa Simone Gouveia Silveira Castro</t>
         </is>
       </c>
       <c r="C101" t="n">
-        <v>53</v>
+        <v>3</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -4744,27 +4744,27 @@
       </c>
       <c r="E101" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Sem instrução</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>Empregador: Sem CNPJ</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>780.189.420-05</t>
+          <t>943.536.610-43</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>669170815</t>
+          <t>619217461</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Coreção gerador de nome de mãe
</commit_message>
<xml_diff>
--- a/perfis_generated_openpyxl.xlsx
+++ b/perfis_generated_openpyxl.xlsx
@@ -479,45 +479,45 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Roberta Nogueira Andrade</t>
+          <t>Giovanni Lopes</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Tatiane Roberta Ferreira d</t>
+          <t>Mariana Sandra Rocha Ribeiro Lopes</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Fundamental completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Desocupado</t>
+          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>340.114.860-51</t>
+          <t>311.492.220-18</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>934150282</t>
+          <t>903704926</t>
         </is>
       </c>
     </row>
@@ -527,25 +527,25 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Felipe Andrade Gonçalves</t>
+          <t>Karla Regina Cavalcanti Rocha</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Tatiane Andrade Machado l</t>
+          <t>Jessica Gouveia Cavalcanti Rocha Regina</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -555,17 +555,17 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>594.655.630-48</t>
+          <t>709.951.750-39</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>381365725</t>
+          <t>986764036</t>
         </is>
       </c>
     </row>
@@ -575,25 +575,25 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Arnaldo Rocha Campos</t>
+          <t>Tatiane Barros</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Valéria Correia Monteiro o</t>
+          <t>Ana Oliveira Barros</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -603,17 +603,17 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>670.260.690-71</t>
+          <t>234.431.350-80</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>992919669</t>
+          <t>139580629</t>
         </is>
       </c>
     </row>
@@ -623,11 +623,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Caio Fernando Lopes</t>
+          <t>Pedro Gouveia Ribeira</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -641,7 +641,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Regina Aline Rocha Fernandes L</t>
+          <t>Rafaela Carolina Gouveia Ribeira</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -656,12 +656,12 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>839.343.820-96</t>
+          <t>131.169.770-54</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>968615717</t>
+          <t>503038146</t>
         </is>
       </c>
     </row>
@@ -671,25 +671,25 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Ronaldo Ribeiro Gouveia</t>
+          <t>Natália Moraes Pires</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Andressa Brenda Araújo Nogueira b</t>
+          <t>Leticia Costa Pires Moraes</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -704,12 +704,12 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>013.678.790-86</t>
+          <t>568.828.350-55</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>739443401</t>
+          <t>445039353</t>
         </is>
       </c>
     </row>
@@ -719,25 +719,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Guilherme Silveira Barbosa</t>
+          <t>Helena Campos</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Isabela Roberta Barros Borges s</t>
+          <t>Brenda Silva Campos</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -747,17 +747,17 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Empregado: Setor privado (sem CLT)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>017.276.640-00</t>
+          <t>501.891.060-77</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>637705131</t>
+          <t>730157861</t>
         </is>
       </c>
     </row>
@@ -767,11 +767,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Thais Isabela Dias</t>
+          <t>Laura Nascimento Santana Alves</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -785,27 +785,27 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Lorena Gouveia Martins a</t>
+          <t>Rosana Alves Nascimento</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Médio completo</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (sem CLT)</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>103.908.370-67</t>
+          <t>135.803.630-69</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>851924260</t>
+          <t>266613963</t>
         </is>
       </c>
     </row>
@@ -815,11 +815,11 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Renata Borges Santos Pereira Alves</t>
+          <t>Elaine Alves Machado</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>49</v>
+        <v>38</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
@@ -833,27 +833,27 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Rafaela Campos o</t>
+          <t>Nathalia Alves Machado</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Médio incompleto</t>
+          <t>Superior incompleto</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Empregado: Setor publico (sem CLT)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>426.510.370-79</t>
+          <t>149.076.830-06</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>071049868</t>
+          <t>366229579</t>
         </is>
       </c>
     </row>
@@ -863,45 +863,45 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Maria Silveira Martins</t>
+          <t>Ricardo Gouveia Andrade</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Roberta Cavalcanti Ribeiro</t>
+          <t>Luiza Gouveia</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Fundamental incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>Desocupado</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>746.308.760-30</t>
+          <t>987.971.870-46</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>824395581</t>
+          <t>455452585</t>
         </is>
       </c>
     </row>
@@ -911,25 +911,25 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Marcelo Campos Santos Monteiro</t>
+          <t>Larissa Cecília Cardoso Martins</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Bianca Cardoso Gonçalves</t>
+          <t>Carolina Cardoso</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -939,17 +939,17 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>395.853.950-53</t>
+          <t>407.675.280-50</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>727571197</t>
+          <t>674898996</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Pequena correção no gerador de número de celular
</commit_message>
<xml_diff>
--- a/perfis_generated_openpyxl.xlsx
+++ b/perfis_generated_openpyxl.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,10 +464,15 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>Celular</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>CPF</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>CEP</t>
         </is>
@@ -479,11 +484,11 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Giovanni Lopes</t>
+          <t>Rafael Hugo Silveira Ribeira Ferreira</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
@@ -497,7 +502,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Mariana Sandra Rocha Ribeiro Lopes</t>
+          <t>Cecília Juliana Ferreira Silveira</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -507,17 +512,22 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>311.492.220-18</t>
+          <t>(48) 97605-3870</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>903704926</t>
+          <t>887.612.030-09</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>921188030</t>
         </is>
       </c>
     </row>
@@ -527,30 +537,30 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Karla Regina Cavalcanti Rocha</t>
+          <t>Carlos Fernando Ribeiro Nunes</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Jessica Gouveia Cavalcanti Rocha Regina</t>
+          <t>Priscila Nunes Fernando</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
@@ -560,12 +570,17 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>709.951.750-39</t>
+          <t>(85) 95121-8739</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>986764036</t>
+          <t>710.090.900-70</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>202427825</t>
         </is>
       </c>
     </row>
@@ -575,11 +590,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Tatiane Barros</t>
+          <t>Lorena Dias</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -588,12 +603,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Ana Oliveira Barros</t>
+          <t>Flávia Monteiro Dias</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -608,12 +623,17 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>234.431.350-80</t>
+          <t>(73) 96202-0181</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>139580629</t>
+          <t>228.714.090-56</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>103240838</t>
         </is>
       </c>
     </row>
@@ -623,11 +643,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Pedro Gouveia Ribeira</t>
+          <t>Hugo Gustavo Ramos Campos</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -636,12 +656,12 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Rafaela Carolina Gouveia Ribeira</t>
+          <t>Sueli Cecília Pereira Campos Gustavo Ramos</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -651,17 +671,22 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>131.169.770-54</t>
+          <t>(92) 99506-7640</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>503038146</t>
+          <t>368.774.670-43</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>251849819</t>
         </is>
       </c>
     </row>
@@ -671,45 +696,50 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Natália Moraes Pires</t>
+          <t>Joaquim Nogueira</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Preto</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Leticia Costa Pires Moraes</t>
+          <t>Carolina Ribeira Nogueira</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Médio incompleto</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Desocupado</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>568.828.350-55</t>
+          <t>(87) 93734-5723</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>445039353</t>
+          <t>991.471.980-52</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>002896322</t>
         </is>
       </c>
     </row>
@@ -719,25 +749,25 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Helena Campos</t>
+          <t>Armando Dias Melo Alves Monteiro</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Brenda Silva Campos</t>
+          <t>Bianca Dias Melo</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -747,17 +777,22 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (sem CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>501.891.060-77</t>
+          <t>(46) 99951-2572</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>730157861</t>
+          <t>914.311.810-05</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>969481242</t>
         </is>
       </c>
     </row>
@@ -767,11 +802,11 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Laura Nascimento Santana Alves</t>
+          <t>Luiza Sandra Alves Andrade Azevedo</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>21</v>
+        <v>49</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
@@ -785,12 +820,12 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Rosana Alves Nascimento</t>
+          <t>Bianca Vanessa Azevedo Sandra Andrade</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
@@ -800,12 +835,17 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>135.803.630-69</t>
+          <t>(53) 96393-7539</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>266613963</t>
+          <t>029.707.070-39</t>
+        </is>
+      </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>687937125</t>
         </is>
       </c>
     </row>
@@ -815,45 +855,50 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Elaine Alves Machado</t>
+          <t>Bruno Sousa</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Outro</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Nathalia Alves Machado</t>
+          <t>Luiza Machado Borges Pires Sousa</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Superior incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Empregado: Setor publico (sem CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>149.076.830-06</t>
+          <t>(48) 98175-6393</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>366229579</t>
+          <t>187.167.750-58</t>
+        </is>
+      </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>227263497</t>
         </is>
       </c>
     </row>
@@ -863,25 +908,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Ricardo Gouveia Andrade</t>
+          <t>Juliana Cavalcanti Pinto Martins</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Luiza Gouveia</t>
+          <t>Nathalia Elaine Pereira Pinto Cavalcanti Martins</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -896,12 +941,17 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>987.971.870-46</t>
+          <t>(44) 98296-7618</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>455452585</t>
+          <t>319.678.350-20</t>
+        </is>
+      </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>179029847</t>
         </is>
       </c>
     </row>
@@ -911,11 +961,11 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Larissa Cecília Cardoso Martins</t>
+          <t>Natália Silveira Cavalcanti</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -924,32 +974,37 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Carolina Cardoso</t>
+          <t>Laura Cavalcanti Silveira</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>407.675.280-50</t>
+          <t>(85) 90785-2366</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>674898996</t>
+          <t>471.400.420-47</t>
+        </is>
+      </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>267793507</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Celular e telefones incluidos
</commit_message>
<xml_diff>
--- a/perfis_generated_openpyxl.xlsx
+++ b/perfis_generated_openpyxl.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,15 +464,20 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>Telefone</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>Celular</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>CPF</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>CEP</t>
         </is>
@@ -484,7 +489,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Rafael Hugo Silveira Ribeira Ferreira</t>
+          <t>Gustavo Ferreira Santana</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -497,12 +502,12 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Cecília Juliana Ferreira Silveira</t>
+          <t>Sueli Borges Santana Ferreira</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -517,17 +522,22 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>(48) 97605-3870</t>
+          <t>53 3566-8652</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>887.612.030-09</t>
+          <t>53 91088-6697</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>921188030</t>
+          <t>934.116.140-13</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>292552690</t>
         </is>
       </c>
     </row>
@@ -537,11 +547,11 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Carlos Fernando Ribeiro Nunes</t>
+          <t>Roberto Gustavo Santos Ribeira</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
@@ -555,32 +565,37 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Priscila Nunes Fernando</t>
+          <t>Carolina Simone Santos Gustavo</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Fundamental incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>(85) 95121-8739</t>
+          <t>97 0757-5038</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>710.090.900-70</t>
+          <t>97 91758-7448</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>202427825</t>
+          <t>952.836.470-56</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>645356793</t>
         </is>
       </c>
     </row>
@@ -590,11 +605,11 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lorena Dias</t>
+          <t>Larissa Tatiana Martins</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
@@ -603,12 +618,12 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Outro</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Flávia Monteiro Dias</t>
+          <t>Flávia Andressa Martins Tatiana</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -618,22 +633,27 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>(73) 96202-0181</t>
+          <t>88 2239-1378</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>228.714.090-56</t>
+          <t>88 93770-1262</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>103240838</t>
+          <t>592.811.940-23</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>660156060</t>
         </is>
       </c>
     </row>
@@ -643,11 +663,11 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Hugo Gustavo Ramos Campos</t>
+          <t>Sérgio Cavalcanti Barros Ribeira Pires</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
@@ -661,12 +681,12 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Sueli Cecília Pereira Campos Gustavo Ramos</t>
+          <t>Rafaela Barros Cavalcanti</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Sem instrução</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
@@ -676,17 +696,22 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>(92) 99506-7640</t>
+          <t>79 4723-9692</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>368.774.670-43</t>
+          <t>79 93616-1771</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>251849819</t>
+          <t>591.100.060-10</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>430784099</t>
         </is>
       </c>
     </row>
@@ -696,11 +721,11 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Joaquim Nogueira</t>
+          <t>Fernando Marcelo Martins</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
@@ -709,37 +734,42 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Preto</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Carolina Ribeira Nogueira</t>
+          <t>Eduarda Pires Martins Marcelo</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Médio incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>(87) 93734-5723</t>
+          <t>34 8557-2628</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>991.471.980-52</t>
+          <t>34 98097-9150</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>002896322</t>
+          <t>542.851.200-89</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>096772649</t>
         </is>
       </c>
     </row>
@@ -749,11 +779,11 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Armando Dias Melo Alves Monteiro</t>
+          <t>Samuel Carvalho</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
@@ -762,12 +792,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Bianca Dias Melo</t>
+          <t>Lorena Pereira Carvalho</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -777,22 +807,27 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Empregado: Setor privado (sem CLT)</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>(46) 99951-2572</t>
+          <t>43 6946-3963</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>914.311.810-05</t>
+          <t>43 99291-6759</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>969481242</t>
+          <t>113.811.910-53</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>219400081</t>
         </is>
       </c>
     </row>
@@ -802,25 +837,25 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Luiza Sandra Alves Andrade Azevedo</t>
+          <t>Miguel Azevedo</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Bianca Vanessa Azevedo Sandra Andrade</t>
+          <t>Isabela Karla Azevedo</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -830,22 +865,27 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Empregado: Setor publico (sem CLT)</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>(53) 96393-7539</t>
+          <t>12 5288-6779</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>029.707.070-39</t>
+          <t>12 96640-9757</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>687937125</t>
+          <t>241.821.300-57</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>064478034</t>
         </is>
       </c>
     </row>
@@ -855,25 +895,25 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Bruno Sousa</t>
+          <t>Márcia Santana Silveira Ribeira</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Outro</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Luiza Machado Borges Pires Sousa</t>
+          <t>Sueli Ribeira Silveira Santana</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -883,22 +923,27 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>(48) 98175-6393</t>
+          <t>55 3579-4968</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>187.167.750-58</t>
+          <t>55 90199-5757</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>227263497</t>
+          <t>572.447.780-74</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>049526582</t>
         </is>
       </c>
     </row>
@@ -908,25 +953,25 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Juliana Cavalcanti Pinto Martins</t>
+          <t>Alexandre Mendes</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Nathalia Elaine Pereira Pinto Cavalcanti Martins</t>
+          <t>Jessica Mendes</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -941,17 +986,22 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>(44) 98296-7618</t>
+          <t>54 0394-6492</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>319.678.350-20</t>
+          <t>54 92238-3698</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>179029847</t>
+          <t>034.705.200-20</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>808547634</t>
         </is>
       </c>
     </row>
@@ -961,50 +1011,55 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Natália Silveira Cavalcanti</t>
+          <t>Vinícius Gonçalves Rodrigues Oliveira</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>54</v>
+        <v>13</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Parda</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Laura Cavalcanti Silveira</t>
+          <t>Tatiana Gonçalves Oliveira Rodrigues</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Fundamental incompleto</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Autonomo: Sem CNPJ</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>(85) 90785-2366</t>
+          <t>69 8126-8908</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>471.400.420-47</t>
+          <t>69 96346-3282</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>267793507</t>
+          <t>459.864.800-74</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>224266837</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Data de aniversário melhorada
</commit_message>
<xml_diff>
--- a/perfis_generated_openpyxl.xlsx
+++ b/perfis_generated_openpyxl.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -439,45 +439,50 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
+          <t>Data de Nascimento</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
           <t>Gênero</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Etnia</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>Nome da Mãe</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>Educação</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Ocupação</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>Telefone</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Celular</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>CPF</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>CEP</t>
         </is>
@@ -489,55 +494,60 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Gustavo Ferreira Santana</t>
+          <t>Andréa Thais Pires</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>27/10/2005</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Sueli Borges Santana Ferreira</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
+          <t>Márcia Thais</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
           <t>Em idade escolar.</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Fora da força de trabalho</t>
-        </is>
-      </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>53 3566-8652</t>
+          <t>Empregado: Setor privado (sem CLT)</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>53 91088-6697</t>
+          <t>73 5858-9702</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>934.116.140-13</t>
+          <t>73 93599-6977</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>292552690</t>
+          <t>819.931.870-81</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>757589557</t>
         </is>
       </c>
     </row>
@@ -547,55 +557,60 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Roberto Gustavo Santos Ribeira</t>
+          <t>Hugo Lopes Gomes</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D3" t="inlineStr">
         <is>
+          <t>21/01/1999</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
           <t>Masculino</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Pardo</t>
-        </is>
-      </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Carolina Simone Santos Gustavo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
+          <t>Patrícia Silva Lopes Gomes</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
           <t>Em idade escolar.</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
-        </is>
-      </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>97 0757-5038</t>
+          <t>Desocupado</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>97 91758-7448</t>
+          <t>97 7172-6076</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>952.836.470-56</t>
+          <t>97 95601-1925</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>645356793</t>
+          <t>559.703.320-46</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>617568248</t>
         </is>
       </c>
     </row>
@@ -605,55 +620,60 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Larissa Tatiana Martins</t>
+          <t>Ana Ribeira Campos Pires Dias</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>30/07/1992</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Feminino</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Outro</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Flávia Andressa Martins Tatiana</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Cristina Pires</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Fundamental completo</t>
         </is>
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>88 2239-1378</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>88 93770-1262</t>
+          <t>84 9500-9043</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>592.811.940-23</t>
+          <t>84 90904-3479</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>660156060</t>
+          <t>797.005.720-99</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>118920320</t>
         </is>
       </c>
     </row>
@@ -663,55 +683,60 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Sérgio Cavalcanti Barros Ribeira Pires</t>
+          <t>Wagner Elias Gomes</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>33</v>
+        <v>1</v>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>11/06/2022</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
           <t>Masculino</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Branco</t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Rafaela Barros Cavalcanti</t>
-        </is>
-      </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Sem instrução</t>
+          <t>Ana Gomes</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Empregado: Setor privado (CLT)</t>
+          <t>Em idade escolar.</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>79 4723-9692</t>
+          <t>Fora da força de trabalho</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>79 93616-1771</t>
+          <t>64 8697-2935</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>591.100.060-10</t>
+          <t>64 94734-0231</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>430784099</t>
+          <t>330.173.150-37</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>857197361</t>
         </is>
       </c>
     </row>
@@ -721,55 +746,60 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Fernando Marcelo Martins</t>
+          <t>Vicente Ribeira Pinto</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="D6" t="inlineStr">
         <is>
+          <t>16/02/1974</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Masculino</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Pardo</t>
-        </is>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Eduarda Pires Martins Marcelo</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Tatiane Leticia Pinto Ribeira</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>34 8557-2628</t>
+          <t>Autonomo: Com CNPJ</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>34 98097-9150</t>
+          <t>31 3328-2454</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>542.851.200-89</t>
+          <t>31 94760-8996</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>096772649</t>
+          <t>635.867.450-10</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>081768997</t>
         </is>
       </c>
     </row>
@@ -779,55 +809,60 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Samuel Carvalho</t>
+          <t>Fábio Ramos Oliveira</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D7" t="inlineStr">
         <is>
+          <t>06/02/2000</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>Masculino</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Branco</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Lorena Pereira Carvalho</t>
+          <t>Pardo</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
+          <t>Isabela Maria Lopes Ramos Oliveira</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
           <t>Em idade escolar.</t>
         </is>
       </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Empregado: Setor privado (sem CLT)</t>
-        </is>
-      </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>43 6946-3963</t>
+          <t>Empregado: Setor ublico (estatutário ou militar)</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>43 99291-6759</t>
+          <t>84 9966-3197</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>113.811.910-53</t>
+          <t>84 90064-3826</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>219400081</t>
+          <t>132.429.830-84</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>406990919</t>
         </is>
       </c>
     </row>
@@ -837,55 +872,60 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Miguel Azevedo</t>
+          <t>Karla Monteiro</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>19/05/1978</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Pardo</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Isabela Karla Azevedo</t>
+          <t>Branca</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>Médio completo</t>
+          <t>Patrícia Monteiro</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>Empregado: Setor publico (sem CLT)</t>
+          <t>Superior completo</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>12 5288-6779</t>
+          <t>Empregado: Trabalhador doméstico (sem CLT)</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>12 96640-9757</t>
+          <t>94 3807-9995</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>241.821.300-57</t>
+          <t>94 99156-7266</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>064478034</t>
+          <t>709.487.240-21</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>454602676</t>
         </is>
       </c>
     </row>
@@ -895,55 +935,60 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Márcia Santana Silveira Ribeira</t>
+          <t>Patrícia Costa</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="D9" t="inlineStr">
         <is>
+          <t>28/05/1981</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
           <t>Feminino</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>Parda</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>Sueli Ribeira Silveira Santana</t>
-        </is>
-      </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Tânia Correia Costa</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
+          <t>Sem instrução</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
           <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
-      <c r="I9" t="inlineStr">
-        <is>
-          <t>55 3579-4968</t>
-        </is>
-      </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>55 90199-5757</t>
+          <t>17 7852-1673</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>572.447.780-74</t>
+          <t>17 96447-0527</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>049526582</t>
+          <t>160.269.100-26</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>855671622</t>
         </is>
       </c>
     </row>
@@ -953,55 +998,60 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Alexandre Mendes</t>
+          <t>Eduarda Oliveira</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>30/04/2001</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Jessica Mendes</t>
+          <t>Parda</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
+          <t>Márcia Oliveira</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
           <t>Em idade escolar.</t>
         </is>
       </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>Fora da força de trabalho</t>
-        </is>
-      </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>54 0394-6492</t>
+          <t>Autonomo: Sem CNPJ</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>54 92238-3698</t>
+          <t>75 3950-9309</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>034.705.200-20</t>
+          <t>75 93548-4325</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>808547634</t>
+          <t>077.496.700-50</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>161352608</t>
         </is>
       </c>
     </row>
@@ -1011,55 +1061,60 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Vinícius Gonçalves Rodrigues Oliveira</t>
+          <t>Cátia Silva Dias</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Masculino</t>
+          <t>10/03/1969</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Branco</t>
+          <t>Feminino</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Tatiana Gonçalves Oliveira Rodrigues</t>
+          <t>Preta</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Amanda Dias</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Fora da força de trabalho</t>
+          <t>Fundamental incompleto</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>69 8126-8908</t>
+          <t>Autonomo: Com CNPJ</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>69 96346-3282</t>
+          <t>28 6071-3312</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>459.864.800-74</t>
+          <t>28 91214-7612</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>224266837</t>
+          <t>804.608.590-13</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>747872635</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ainda falta corrigir o Update
</commit_message>
<xml_diff>
--- a/perfis_generated_openpyxl.xlsx
+++ b/perfis_generated_openpyxl.xlsx
@@ -489,55 +489,55 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Cecília Monteiro Pinto</t>
+          <t>Diego Ramos Barros</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>07/02/2002</t>
+          <t>05/03/1995</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Feminino</t>
+          <t>Masculino</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Branca</t>
+          <t>Branco</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Em idade escolar.</t>
+          <t>Médio completo</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Autônomo: Sem CNPJ</t>
+          <t>Empregado: Setor privado (CLT)</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>(12) 7342-9189</t>
+          <t>(41) 1417-2308</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>(12) 95146-1408</t>
+          <t>(41) 98806-7654</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>054.663.600-40</t>
+          <t>099.959.210-65</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>741258623</t>
+          <t>694640277</t>
         </is>
       </c>
     </row>

</xml_diff>